<commit_message>
reset position for all scene
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Scene.xlsx
+++ b/_Out/NFDataCfg/Excel/Scene.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>Id</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>../NFDataCfg/Ini/Scene/1.xml</t>
-  </si>
-  <si>
-    <t>100,114,0</t>
   </si>
   <si>
     <t>Sources/Music/Town</t>
@@ -235,6 +232,21 @@
     <t>NORMAL,
 SINGLE_CLONE_SCENE,
 MULTI_CLONE_SCENE, TYPE_GUILD</t>
+  </si>
+  <si>
+    <t>89,104,0</t>
+  </si>
+  <si>
+    <t>89,102,0</t>
+  </si>
+  <si>
+    <t>100,115,0</t>
+  </si>
+  <si>
+    <t>95,102,0</t>
+  </si>
+  <si>
+    <t>88,105,0</t>
   </si>
 </sst>
 </file>
@@ -823,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -892,7 +904,7 @@
         <v>13</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1">
@@ -1197,7 +1209,7 @@
     </row>
     <row r="8" spans="1:16" s="16" customFormat="1">
       <c r="A8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="16">
         <v>0</v>
@@ -1323,7 +1335,7 @@
         <v>9</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>30</v>
@@ -1332,7 +1344,7 @@
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1354,44 +1366,44 @@
       <c r="F11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>34</v>
+      <c r="G11" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="H11">
         <v>500</v>
       </c>
       <c r="I11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" s="13" t="s">
+      <c r="N11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="O11" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="P11" s="19"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12">
         <v>1000</v>
@@ -1400,16 +1412,16 @@
         <v>50</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="H12">
         <v>500</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1421,25 +1433,25 @@
         <v>0</v>
       </c>
       <c r="M12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="N12" s="12" t="s">
+      <c r="O12" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="P12" s="19"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13">
         <v>1000</v>
@@ -1448,16 +1460,16 @@
         <v>50</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="H13">
         <v>500</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1469,25 +1481,25 @@
         <v>0</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O13" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="P13" s="19"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>1000</v>
@@ -1496,16 +1508,16 @@
         <v>50</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="H14">
         <v>500</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1517,25 +1529,25 @@
         <v>0</v>
       </c>
       <c r="M14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="O14" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="P14" s="19"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <v>1000</v>
@@ -1544,16 +1556,16 @@
         <v>50</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="H15">
         <v>500</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1565,25 +1577,25 @@
         <v>0</v>
       </c>
       <c r="M15" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="N15" s="12" t="s">
+      <c r="O15" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="O15" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="P15" s="19"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
         <v>56</v>
       </c>
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16">
         <v>1000</v>
@@ -1592,16 +1604,16 @@
         <v>50</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="H16">
         <v>500</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1613,13 +1625,13 @@
         <v>0</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="P16" s="19"/>
     </row>

</xml_diff>